<commit_message>
UT edit to DACD
</commit_message>
<xml_diff>
--- a/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
+++ b/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.1.2\InputData\geoeng\DACD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-texas\InputData\geoeng\DACD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB89F9-AA00-47A5-A09D-D6F9F4A41987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5445" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="116">
   <si>
     <t>Sources:</t>
   </si>
@@ -316,9 +315,6 @@
     <t>https://www.sciencedirect.com/science/article/pii/S0959652619307772</t>
   </si>
   <si>
-    <t>Here's an alternative source to consider (by Fasihi)</t>
-  </si>
-  <si>
     <t>this source was published in the same month as the one EPS cites (by Realmonte), but it is more bullish about DAC costs and adoption</t>
   </si>
   <si>
@@ -328,9 +324,6 @@
     <t>the Fasihi study assumes a bit more DAC adoption and costs that get lower over time.</t>
   </si>
   <si>
-    <t xml:space="preserve">Realmonte Adoption (DAC1 Mtco2/yr) </t>
-  </si>
-  <si>
     <t>These studies both look at technologies that "ues water solutions containing hydroxide sorbents", which Realmonte calls "DAC1" and Fasihi calls "HT" (high temperature). These are the technologies described below.</t>
   </si>
   <si>
@@ -349,111 +342,60 @@
     <t>larger scale, uses water solutions containing hydroxide sorbents, requires high input heat which usually means burning fuels like natural gas</t>
   </si>
   <si>
-    <t xml:space="preserve">EPS only uses the Realmonte Study, but we will average the results of both studies to get something more averaged out. It turns out that Realmonte seems a bit conservative while Fasihi may be a bit optimistic. Given the large </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uncertainty in DACs, it seems prudent to consider both and take their average. </t>
-  </si>
-  <si>
     <t>Note that Fasihi uses 2018 Euros using a constant 1.33 USD conversion rate. So, to convert from thes 2018 Euros to 2012 USD, we multiply by (1.33*0.91)</t>
   </si>
   <si>
-    <t>Fasihi (Table 6) Cap Cost $/ton (Base Case)</t>
-  </si>
-  <si>
-    <t>Fasihi (Table 6) Cap Cost $/ton (Conservative)</t>
-  </si>
-  <si>
-    <t>Fasihi (Table 6) Cap Cost $/ton (Average)</t>
-  </si>
-  <si>
-    <t>Adoption Rate / Global DACs Demand</t>
-  </si>
-  <si>
-    <t>Fasihi (Table 5) Adoption (Mtco2/yr) (Base Case)</t>
-  </si>
-  <si>
     <t>Fasihi (Table 5) Adoption (Mtco2/yr) (Conservative)</t>
   </si>
   <si>
-    <t>Fasihi (Table 5) Adoption (Mtco2/yr) (Average)</t>
-  </si>
-  <si>
-    <t>Note that Fasihi has "conservative" and "base case" scenarios and Realmonte often gives "high" and "low" numbers. We take the average in both cases.</t>
-  </si>
-  <si>
-    <t>Realmonte Cap Cost $/ton (High case)</t>
-  </si>
-  <si>
-    <t>Realmonte Cap Cost $/ton (Low case)</t>
-  </si>
-  <si>
-    <t>Realmonte Cap Cost $/ton (Average)</t>
-  </si>
-  <si>
-    <t>Realmonte Electricity GJ/ton (Low case)</t>
-  </si>
-  <si>
-    <t>Realmonte Electricity GJ/ton (High case)</t>
-  </si>
-  <si>
-    <t>Realmonte Electricity GJ/ton (Average)</t>
-  </si>
-  <si>
-    <t>Realmonte Heat GJ/ton (Low case)</t>
-  </si>
-  <si>
-    <t>Realmonte Heat GJ/ton (High case)</t>
-  </si>
-  <si>
-    <t>Realmonte Heat GJ/ton (Average)</t>
-  </si>
-  <si>
     <t>Fasihi also provides a good argument that DAC technology calculations should focus on electrification. That is, when gas or hydrogen is used for the input heat, the sustainability or energy intensity become unattractive.</t>
   </si>
   <si>
-    <t>So we will convert Realmonte's numbers, which assume nutural gas as the heat input, into electricity only.</t>
-  </si>
-  <si>
-    <t>Realmonte Electricity btu/ton (Average)</t>
-  </si>
-  <si>
-    <t>Realmonte Heat btu/ton (Average)</t>
-  </si>
-  <si>
-    <t>Realmonte Total btu/ton (Average)</t>
-  </si>
-  <si>
     <t>Fasihi (Table 7) Energy kWh/ton</t>
   </si>
   <si>
     <t>Fasihi (Table 7) Energy btu/ton</t>
   </si>
   <si>
-    <t>Average btu/ton</t>
-  </si>
-  <si>
-    <t>Average $/ton</t>
-  </si>
-  <si>
-    <t>Average Mt/year</t>
-  </si>
-  <si>
     <t>DAC1/HT: can use natural gas for heat, but we assume it will be electrified</t>
   </si>
   <si>
     <t>Texas Average Mt/year</t>
+  </si>
+  <si>
+    <t>Here's an alternative source (by Fasihi) which is also used by the WISdom model.</t>
+  </si>
+  <si>
+    <t>Both WISdom and EPS assume that DACs capital cost and energy efficiency remain constant over time. We will do the same.</t>
+  </si>
+  <si>
+    <t>So, we will take the 2020 numbers for the studies and assume that they are constant through 2050.</t>
+  </si>
+  <si>
+    <t>We will assum that DACS do not use natural gas for heat, but that they are completely electrified. Based on that assumption, we will use the Fasihi study because it makes the same assumption (while Realmonte uses gas for DACs heat).</t>
+  </si>
+  <si>
+    <t>Note that Fasihi has "conservative" and "base case" scenarios. Given the uncertainty around DACs as a future tech, we will use the conservative numbers.</t>
+  </si>
+  <si>
+    <t>Constant $/ton for EPS model</t>
+  </si>
+  <si>
+    <t>Fasihi (Table 6) Cap Cost 2012$/ton (Conservative)</t>
+  </si>
+  <si>
+    <t>Constant btu/ton for EPS model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,12 +456,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -567,7 +503,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -591,30 +527,25 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1001,35 +932,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" customWidth="1"/>
+    <col min="2" max="2" width="47.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1037,105 +968,105 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1143,48 +1074,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="8" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" customWidth="1"/>
+    <col min="2" max="8" width="11.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>82</v>
       </c>
@@ -1195,7 +1126,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1148,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,7 +1159,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1239,12 +1170,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1255,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1266,7 +1197,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1277,17 +1208,17 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1309,7 +1240,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1320,39 +1251,39 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
         <v>44</v>
       </c>
@@ -1364,27 +1295,27 @@
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B57">
         <v>2045</v>
       </c>
@@ -1407,7 +1338,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -1433,7 +1364,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -1459,7 +1390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -1467,7 +1398,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B63">
         <v>2045</v>
       </c>
@@ -1490,7 +1421,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>33</v>
       </c>
@@ -1523,7 +1454,7 @@
         <v>27.071428571428573</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -1556,27 +1487,27 @@
         <v>2.8571428571428568</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -1590,7 +1521,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -1604,7 +1535,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>43</v>
       </c>
@@ -1613,7 +1544,7 @@
         <v>0.24237500000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="5" t="s">
         <v>45</v>
       </c>
@@ -1625,7 +1556,7 @@
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B77">
         <v>2045</v>
       </c>
@@ -1648,7 +1579,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>33</v>
       </c>
@@ -1681,7 +1612,7 @@
         <v>6.5614375000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>34</v>
       </c>
@@ -1714,12 +1645,12 @@
         <v>0.69249999999999989</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B82">
         <v>2045</v>
       </c>
@@ -1742,7 +1673,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -1775,7 +1706,7 @@
         <v>6561437500</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -1808,32 +1739,32 @@
         <v>692499999.99999988</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -1841,7 +1772,7 @@
         <v>947086</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -1857,818 +1788,383 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C686EB8-A5A6-4682-9510-E2AB00CB780B}">
-  <dimension ref="A1:J59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" customWidth="1"/>
-    <col min="2" max="8" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.265625" customWidth="1"/>
+    <col min="2" max="8" width="11.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="20" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
         <v>99</v>
       </c>
-      <c r="B8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>124</v>
-      </c>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="4"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>133</v>
-      </c>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B19" s="1"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="4"/>
+      <c r="B20">
+        <v>2020</v>
+      </c>
+      <c r="C20">
+        <v>2030</v>
+      </c>
+      <c r="D20">
+        <v>2040</v>
+      </c>
+      <c r="E20">
+        <v>2050</v>
+      </c>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21">
-        <v>2020</v>
-      </c>
-      <c r="C21">
-        <v>2030</v>
-      </c>
-      <c r="D21">
-        <v>2040</v>
-      </c>
-      <c r="E21">
-        <v>2050</v>
-      </c>
-      <c r="F21">
-        <v>2060</v>
-      </c>
-      <c r="G21">
-        <v>2100</v>
-      </c>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="26">
-        <v>180</v>
-      </c>
-      <c r="C22" s="26">
-        <v>180</v>
-      </c>
-      <c r="D22" s="26">
-        <v>180</v>
-      </c>
-      <c r="E22" s="26">
-        <v>180</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26">
-        <v>100</v>
-      </c>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B23" s="26">
-        <v>300</v>
-      </c>
-      <c r="C23" s="26">
-        <v>300</v>
-      </c>
-      <c r="D23" s="26">
-        <v>300</v>
-      </c>
-      <c r="E23" s="26">
-        <v>300</v>
-      </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26">
-        <v>100</v>
-      </c>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24">
-        <f>AVERAGE(B22:B23)</f>
-        <v>240</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:G24" si="0">AVERAGE(C22:C23)</f>
-        <v>240</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="24">
+      <c r="B21" s="22">
         <f>815*(1.33*0.91)</f>
         <v>986.39450000000011</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C21" s="22">
         <f>378*(1.33*0.91)</f>
         <v>457.49340000000007</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D21" s="22">
         <f>265*(1.33*0.91)</f>
         <v>320.72950000000003</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E21" s="22">
         <f>222*(1.33*0.91)</f>
         <v>268.68660000000006</v>
       </c>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="26">
+        <f>B21</f>
+        <v>986.39450000000011</v>
+      </c>
+      <c r="C22" s="26">
+        <f>B21</f>
+        <v>986.39450000000011</v>
+      </c>
+      <c r="D22" s="26">
+        <f>B21</f>
+        <v>986.39450000000011</v>
+      </c>
+      <c r="E22" s="26">
+        <f>B21</f>
+        <v>986.39450000000011</v>
+      </c>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="14">
+        <v>1535</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1458</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1385</v>
+      </c>
+      <c r="E24" s="14">
+        <v>1316</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="14">
+        <f>B24*3412</f>
+        <v>5237420</v>
+      </c>
+      <c r="C25" s="14">
+        <f>C24*3412</f>
+        <v>4974696</v>
+      </c>
+      <c r="D25" s="14">
+        <f>D24*3412</f>
+        <v>4725620</v>
+      </c>
+      <c r="E25" s="14">
+        <f>E24*3412</f>
+        <v>4490192</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="14">
+        <f>B25</f>
+        <v>5237420</v>
+      </c>
+      <c r="C26" s="14">
+        <f>B25</f>
+        <v>5237420</v>
+      </c>
+      <c r="D26" s="14">
+        <f>B25</f>
+        <v>5237420</v>
+      </c>
+      <c r="E26" s="14">
+        <f>B25</f>
+        <v>5237420</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="25"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="C28" s="22">
+        <v>236.5</v>
+      </c>
+      <c r="D28" s="22">
+        <v>2395.5</v>
+      </c>
+      <c r="E28" s="22">
+        <v>7678</v>
+      </c>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="20"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1.6688000000000001</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35">
+        <v>2017</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36">
+        <v>2017</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="10">
+        <f>C35/C36</f>
+        <v>2.086E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="24">
-        <f>815*(1.33*0.91)</f>
-        <v>986.39450000000011</v>
-      </c>
-      <c r="C26" s="24">
-        <f>211*(1.33*0.91)</f>
-        <v>255.37330000000003</v>
-      </c>
-      <c r="D26" s="24">
-        <f>122*(1.33*0.91)</f>
-        <v>147.65660000000003</v>
-      </c>
-      <c r="E26" s="24">
-        <f>93*(1.33*0.91)</f>
-        <v>112.55790000000002</v>
-      </c>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="14">
-        <f>AVERAGE(B25:B26)</f>
-        <v>986.39450000000011</v>
-      </c>
-      <c r="C27" s="14">
-        <f t="shared" ref="C27:E27" si="1">AVERAGE(C25:C26)</f>
-        <v>356.43335000000002</v>
-      </c>
-      <c r="D27" s="14">
-        <f t="shared" si="1"/>
-        <v>234.19305000000003</v>
-      </c>
-      <c r="E27" s="14">
-        <f t="shared" si="1"/>
-        <v>190.62225000000004</v>
-      </c>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="B28" s="29">
-        <f>AVERAGE(B27,B24)</f>
-        <v>613.19725000000005</v>
-      </c>
-      <c r="C28" s="29">
-        <f t="shared" ref="C28:E28" si="2">AVERAGE(C27,C24)</f>
-        <v>298.21667500000001</v>
-      </c>
-      <c r="D28" s="29">
-        <f t="shared" si="2"/>
-        <v>237.09652500000001</v>
-      </c>
-      <c r="E28" s="29">
-        <f t="shared" si="2"/>
-        <v>215.311125</v>
-      </c>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J29" s="6"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B30" s="8">
-        <v>1.3</v>
-      </c>
-      <c r="C30" s="8">
-        <v>1.3</v>
-      </c>
-      <c r="D30" s="8">
-        <v>1.3</v>
-      </c>
-      <c r="E30" s="8">
-        <v>1.3</v>
-      </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="8">
-        <v>1.8</v>
-      </c>
-      <c r="C31" s="8">
-        <v>1.8</v>
-      </c>
-      <c r="D31" s="8">
-        <v>1.8</v>
-      </c>
-      <c r="E31" s="8">
-        <v>1.8</v>
-      </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="8">
-        <f>AVERAGE(B30:B31)</f>
-        <v>1.55</v>
-      </c>
-      <c r="C32" s="8">
-        <f t="shared" ref="C32:E32" si="3">AVERAGE(C30:C31)</f>
-        <v>1.55</v>
-      </c>
-      <c r="D32" s="8">
-        <f t="shared" si="3"/>
-        <v>1.55</v>
-      </c>
-      <c r="E32" s="8">
-        <f t="shared" si="3"/>
-        <v>1.55</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="14">
-        <f>B32*947817</f>
-        <v>1469116.35</v>
-      </c>
-      <c r="C33" s="14">
-        <f t="shared" ref="C33:E33" si="4">C32*947817</f>
-        <v>1469116.35</v>
-      </c>
-      <c r="D33" s="14">
-        <f t="shared" si="4"/>
-        <v>1469116.35</v>
-      </c>
-      <c r="E33" s="14">
-        <f t="shared" si="4"/>
-        <v>1469116.35</v>
-      </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="8">
-        <v>5.3</v>
-      </c>
-      <c r="C34" s="8">
-        <v>5.3</v>
-      </c>
-      <c r="D34" s="8">
-        <v>5.3</v>
-      </c>
-      <c r="E34" s="8">
-        <v>5.3</v>
-      </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="8">
-        <v>8.1</v>
-      </c>
-      <c r="C35" s="8">
-        <v>8.1</v>
-      </c>
-      <c r="D35" s="8">
-        <v>8.1</v>
-      </c>
-      <c r="E35" s="8">
-        <v>8.1</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B36" s="8">
-        <f>AVERAGE(B34:B35)</f>
-        <v>6.6999999999999993</v>
-      </c>
-      <c r="C36" s="8">
-        <f t="shared" ref="C36" si="5">AVERAGE(C34:C35)</f>
-        <v>6.6999999999999993</v>
-      </c>
-      <c r="D36" s="8">
-        <f t="shared" ref="D36" si="6">AVERAGE(D34:D35)</f>
-        <v>6.6999999999999993</v>
-      </c>
-      <c r="E36" s="8">
-        <f t="shared" ref="E36" si="7">AVERAGE(E34:E35)</f>
-        <v>6.6999999999999993</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" s="14">
-        <f>B36*947817</f>
-        <v>6350373.8999999994</v>
-      </c>
-      <c r="C37" s="14">
-        <f t="shared" ref="C37:E37" si="8">C36*947817</f>
-        <v>6350373.8999999994</v>
-      </c>
-      <c r="D37" s="14">
-        <f t="shared" si="8"/>
-        <v>6350373.8999999994</v>
-      </c>
-      <c r="E37" s="14">
-        <f t="shared" si="8"/>
-        <v>6350373.8999999994</v>
-      </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="14">
-        <f>SUM(B37,B33)</f>
-        <v>7819490.25</v>
-      </c>
-      <c r="C38" s="14">
-        <f t="shared" ref="C38:E38" si="9">SUM(C37,C33)</f>
-        <v>7819490.25</v>
-      </c>
-      <c r="D38" s="14">
-        <f t="shared" si="9"/>
-        <v>7819490.25</v>
-      </c>
-      <c r="E38" s="14">
-        <f t="shared" si="9"/>
-        <v>7819490.25</v>
-      </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="14">
-        <v>1535</v>
-      </c>
-      <c r="C39" s="14">
-        <v>1458</v>
-      </c>
-      <c r="D39" s="14">
-        <v>1385</v>
-      </c>
-      <c r="E39" s="14">
-        <v>1316</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B40" s="14">
-        <f>B39*3412</f>
-        <v>5237420</v>
-      </c>
-      <c r="C40" s="14">
-        <f t="shared" ref="C40:E40" si="10">C39*3412</f>
-        <v>4974696</v>
-      </c>
-      <c r="D40" s="14">
-        <f t="shared" si="10"/>
-        <v>4725620</v>
-      </c>
-      <c r="E40" s="14">
-        <f t="shared" si="10"/>
-        <v>4490192</v>
-      </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="B41" s="14">
-        <f>AVERAGE(B40,B38)</f>
-        <v>6528455.125</v>
-      </c>
-      <c r="C41" s="14">
-        <f t="shared" ref="C41:E41" si="11">AVERAGE(C40,C38)</f>
-        <v>6397093.125</v>
-      </c>
-      <c r="D41" s="14">
-        <f t="shared" si="11"/>
-        <v>6272555.125</v>
-      </c>
-      <c r="E41" s="14">
-        <f t="shared" si="11"/>
-        <v>6154841.125</v>
-      </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="14">
-        <v>0</v>
-      </c>
-      <c r="C44" s="14">
-        <v>0</v>
-      </c>
-      <c r="D44" s="14">
-        <v>0</v>
-      </c>
-      <c r="E44" s="14">
-        <v>400</v>
-      </c>
-      <c r="F44">
-        <v>1500</v>
-      </c>
-      <c r="G44" s="14">
-        <v>30000</v>
-      </c>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" s="24">
-        <v>3</v>
-      </c>
-      <c r="C45" s="24">
-        <v>473</v>
-      </c>
-      <c r="D45" s="24">
-        <v>4791</v>
-      </c>
-      <c r="E45" s="24">
-        <v>15356</v>
-      </c>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B46" s="27">
-        <f>B45*0.5</f>
-        <v>1.5</v>
-      </c>
-      <c r="C46" s="24">
-        <f t="shared" ref="C46:E46" si="12">C45*0.5</f>
-        <v>236.5</v>
-      </c>
-      <c r="D46" s="24">
-        <f t="shared" si="12"/>
-        <v>2395.5</v>
-      </c>
-      <c r="E46" s="24">
-        <f t="shared" si="12"/>
-        <v>7678</v>
-      </c>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="J46" s="6"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="19">
-        <f>AVERAGE(B45:B46)</f>
-        <v>2.25</v>
-      </c>
-      <c r="C47" s="14">
-        <f t="shared" ref="C47:E47" si="13">AVERAGE(C45:C46)</f>
-        <v>354.75</v>
-      </c>
-      <c r="D47" s="14">
-        <f t="shared" si="13"/>
-        <v>3593.25</v>
-      </c>
-      <c r="E47" s="14">
-        <f t="shared" si="13"/>
-        <v>11517</v>
-      </c>
-      <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="14">
-        <f>AVERAGE(B47,B44)</f>
-        <v>1.125</v>
-      </c>
-      <c r="C48" s="14">
-        <f t="shared" ref="C48:E48" si="14">AVERAGE(C47,C44)</f>
-        <v>177.375</v>
-      </c>
-      <c r="D48" s="14">
-        <f t="shared" si="14"/>
-        <v>1796.625</v>
-      </c>
-      <c r="E48" s="14">
-        <f t="shared" si="14"/>
-        <v>5958.5</v>
-      </c>
-      <c r="J48" s="6"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="J49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="20">
-        <v>1.6688000000000001</v>
-      </c>
-      <c r="D55" t="s">
-        <v>41</v>
-      </c>
-      <c r="E55">
-        <v>2017</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56">
-        <v>80</v>
-      </c>
-      <c r="D56" t="s">
-        <v>42</v>
-      </c>
-      <c r="E56">
-        <v>2017</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" s="10">
-        <f>C55/C56</f>
-        <v>2.086E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" s="32">
-        <f>B48*$C$57</f>
-        <v>2.3467499999999999E-2</v>
-      </c>
-      <c r="C59" s="32">
-        <f t="shared" ref="C59:E59" si="15">C48*$C$57</f>
-        <v>3.7000424999999999</v>
-      </c>
-      <c r="D59" s="32">
-        <f t="shared" si="15"/>
-        <v>37.477597500000002</v>
-      </c>
-      <c r="E59" s="32">
-        <f t="shared" si="15"/>
-        <v>124.29431</v>
-      </c>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
+      <c r="B39" s="28">
+        <f>B28*$C$37</f>
+        <v>3.1289999999999998E-2</v>
+      </c>
+      <c r="C39" s="28">
+        <f t="shared" ref="C39:E39" si="0">C28*$C$37</f>
+        <v>4.9333900000000002</v>
+      </c>
+      <c r="D39" s="28">
+        <f t="shared" si="0"/>
+        <v>49.970129999999997</v>
+      </c>
+      <c r="E39" s="28">
+        <f t="shared" si="0"/>
+        <v>160.16308000000001</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{45DD5CF1-C46A-42D6-A7D7-A22A80577B18}"/>
-    <hyperlink ref="G56" r:id="rId2" xr:uid="{89957D1A-BCF1-498F-B397-AE2ACF2DE8B9}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="G36" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2676,27 +2172,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:N2"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" customWidth="1"/>
+    <col min="15" max="15" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="33" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -2803,7 +2299,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -2817,128 +2313,128 @@
         <v>0</v>
       </c>
       <c r="E2" s="14">
-        <f>'Texas Data'!B59*1000000</f>
-        <v>23467.5</v>
+        <f>'Texas Data'!B39*1000000</f>
+        <v>31290</v>
       </c>
       <c r="F2" s="14">
         <f>0.9*E2+0.1*O2</f>
-        <v>391125</v>
+        <v>521500</v>
       </c>
       <c r="G2" s="14">
         <f>0.8*E2+0.2*O2</f>
-        <v>758782.5</v>
+        <v>1011710</v>
       </c>
       <c r="H2" s="14">
         <f>0.7*E2+0.3*O2</f>
-        <v>1126440</v>
+        <v>1501920</v>
       </c>
       <c r="I2" s="14">
         <f>0.6*E2+0.4*O2</f>
-        <v>1494097.5</v>
+        <v>1992130</v>
       </c>
       <c r="J2" s="14">
         <f>0.5*E2+0.5*O2</f>
-        <v>1861755</v>
+        <v>2482340</v>
       </c>
       <c r="K2" s="14">
         <f>0.4*E2+0.6*O2</f>
-        <v>2229412.5</v>
+        <v>2972550</v>
       </c>
       <c r="L2" s="14">
         <f>0.3*E2+0.7*O2</f>
-        <v>2597070</v>
+        <v>3462760</v>
       </c>
       <c r="M2" s="14">
         <f>0.2*E2+0.8*O2</f>
-        <v>2964727.5</v>
+        <v>3952970</v>
       </c>
       <c r="N2" s="14">
         <f>0.1*E2+0.9*O2</f>
-        <v>3332385</v>
+        <v>4443180</v>
       </c>
       <c r="O2" s="14">
-        <f>'Texas Data'!C59*1000000</f>
-        <v>3700042.5</v>
+        <f>'Texas Data'!C39*1000000</f>
+        <v>4933390</v>
       </c>
       <c r="P2" s="14">
         <f>0.9*O2+0.1*Y2</f>
-        <v>7077798</v>
+        <v>9437064</v>
       </c>
       <c r="Q2" s="14">
         <f>0.8*O2+0.2*Y2</f>
-        <v>10455553.5</v>
+        <v>13940738</v>
       </c>
       <c r="R2" s="14">
         <f>0.7*O2+0.3*Y2</f>
-        <v>13833309</v>
+        <v>18444412</v>
       </c>
       <c r="S2" s="14">
         <f>0.6*O2+0.4*Y2</f>
-        <v>17211064.5</v>
+        <v>22948086</v>
       </c>
       <c r="T2" s="14">
         <f>0.5*O2+0.5*Y2</f>
-        <v>20588820</v>
+        <v>27451760</v>
       </c>
       <c r="U2" s="14">
         <f>0.4*O2+0.6*Y2</f>
-        <v>23966575.5</v>
+        <v>31955434</v>
       </c>
       <c r="V2" s="14">
         <f>0.3*O2+0.7*Y2</f>
-        <v>27344331</v>
+        <v>36459108</v>
       </c>
       <c r="W2" s="14">
         <f>0.2*O2+0.8*Y2</f>
-        <v>30722086.5</v>
+        <v>40962782</v>
       </c>
       <c r="X2" s="14">
         <f>0.1*O2+0.9*Y2</f>
-        <v>34099842</v>
+        <v>45466456</v>
       </c>
       <c r="Y2" s="14">
-        <f>'Texas Data'!D59*1000000</f>
-        <v>37477597.5</v>
+        <f>'Texas Data'!D39*1000000</f>
+        <v>49970130</v>
       </c>
       <c r="Z2" s="14">
         <f>0.9*Y2+0.1*AI2</f>
-        <v>46159268.75</v>
+        <v>60989425</v>
       </c>
       <c r="AA2" s="14">
         <f>0.8*Y2+0.2*AI2</f>
-        <v>54840940</v>
+        <v>72008720</v>
       </c>
       <c r="AB2" s="14">
         <f>0.7*Y2+0.3*AI2</f>
-        <v>63522611.25</v>
+        <v>83028015</v>
       </c>
       <c r="AC2" s="14">
         <f>0.6*Y2+0.4*AI2</f>
-        <v>72204282.5</v>
+        <v>94047310</v>
       </c>
       <c r="AD2" s="14">
         <f>0.5*Y2+0.5*AI2</f>
-        <v>80885953.75</v>
+        <v>105066605</v>
       </c>
       <c r="AE2" s="14">
         <f>0.4*Y2+0.6*AI2</f>
-        <v>89567625</v>
+        <v>116085900</v>
       </c>
       <c r="AF2" s="14">
         <f>0.3*Y2+0.7*AI2</f>
-        <v>98249296.25</v>
+        <v>127105195</v>
       </c>
       <c r="AG2" s="14">
         <f>0.2*Y2+0.8*AI2</f>
-        <v>106930967.5</v>
+        <v>138124490</v>
       </c>
       <c r="AH2" s="14">
         <f>0.1*Y2+0.9*AI2</f>
-        <v>115612638.75</v>
+        <v>149143785</v>
       </c>
       <c r="AI2">
-        <f>'Texas Data'!E59*1000000</f>
-        <v>124294310</v>
+        <f>'Texas Data'!E39*1000000</f>
+        <v>160163080</v>
       </c>
     </row>
   </sheetData>
@@ -2947,23 +2443,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:N2"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -3070,148 +2566,148 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="14">
         <f t="shared" ref="B2:C2" si="0">C2</f>
-        <v>6528455.125</v>
+        <v>5237420</v>
       </c>
       <c r="C2" s="14">
         <f t="shared" si="0"/>
-        <v>6528455.125</v>
+        <v>5237420</v>
       </c>
       <c r="D2" s="14">
         <f>E2</f>
-        <v>6528455.125</v>
+        <v>5237420</v>
       </c>
       <c r="E2" s="14">
-        <f>'Texas Data'!B41</f>
-        <v>6528455.125</v>
+        <f>'Texas Data'!B26</f>
+        <v>5237420</v>
       </c>
       <c r="F2" s="14">
         <f>0.9*E2+0.1*O2</f>
-        <v>6515318.9249999998</v>
+        <v>5237420</v>
       </c>
       <c r="G2" s="14">
         <f>0.8*E2+0.2*O2</f>
-        <v>6502182.7250000006</v>
+        <v>5237420</v>
       </c>
       <c r="H2" s="14">
         <f>0.7*E2+0.3*O2</f>
-        <v>6489046.5249999994</v>
+        <v>5237420</v>
       </c>
       <c r="I2" s="14">
         <f>0.6*E2+0.4*O2</f>
-        <v>6475910.3249999993</v>
+        <v>5237420</v>
       </c>
       <c r="J2" s="14">
         <f>0.5*E2+0.5*O2</f>
-        <v>6462774.125</v>
+        <v>5237420</v>
       </c>
       <c r="K2" s="14">
         <f>0.4*E2+0.6*O2</f>
-        <v>6449637.9250000007</v>
+        <v>5237420</v>
       </c>
       <c r="L2" s="14">
         <f>0.3*E2+0.7*O2</f>
-        <v>6436501.7249999996</v>
+        <v>5237420</v>
       </c>
       <c r="M2" s="14">
         <f>0.2*E2+0.8*O2</f>
-        <v>6423365.5250000004</v>
+        <v>5237420</v>
       </c>
       <c r="N2" s="14">
         <f>0.1*E2+0.9*O2</f>
-        <v>6410229.3250000002</v>
+        <v>5237420</v>
       </c>
       <c r="O2" s="14">
-        <f>'Texas Data'!C41</f>
-        <v>6397093.125</v>
+        <f>'Texas Data'!C26</f>
+        <v>5237420</v>
       </c>
       <c r="P2" s="14">
         <f>0.9*O2+0.1*Y2</f>
-        <v>6384639.3250000002</v>
+        <v>5237420</v>
       </c>
       <c r="Q2" s="14">
         <f>0.8*O2+0.2*Y2</f>
-        <v>6372185.5250000004</v>
+        <v>5237420</v>
       </c>
       <c r="R2" s="14">
         <f>0.7*O2+0.3*Y2</f>
-        <v>6359731.7249999996</v>
+        <v>5237420</v>
       </c>
       <c r="S2" s="14">
         <f>0.6*O2+0.4*Y2</f>
-        <v>6347277.9250000007</v>
+        <v>5237420</v>
       </c>
       <c r="T2" s="14">
         <f>0.5*O2+0.5*Y2</f>
-        <v>6334824.125</v>
+        <v>5237420</v>
       </c>
       <c r="U2" s="14">
         <f>0.4*O2+0.6*Y2</f>
-        <v>6322370.3249999993</v>
+        <v>5237420</v>
       </c>
       <c r="V2" s="14">
         <f>0.3*O2+0.7*Y2</f>
-        <v>6309916.5249999994</v>
+        <v>5237420</v>
       </c>
       <c r="W2" s="14">
         <f>0.2*O2+0.8*Y2</f>
-        <v>6297462.7250000006</v>
+        <v>5237420</v>
       </c>
       <c r="X2" s="14">
         <f>0.1*O2+0.9*Y2</f>
-        <v>6285008.9249999998</v>
+        <v>5237420</v>
       </c>
       <c r="Y2" s="14">
-        <f>'Texas Data'!D41</f>
-        <v>6272555.125</v>
+        <f>'Texas Data'!D26</f>
+        <v>5237420</v>
       </c>
       <c r="Z2" s="14">
         <f>0.9*Y2+0.1*AI2</f>
-        <v>6260783.7249999996</v>
+        <v>5237420</v>
       </c>
       <c r="AA2" s="14">
         <f>0.8*Y2+0.2*AI2</f>
-        <v>6249012.3250000011</v>
+        <v>5237420</v>
       </c>
       <c r="AB2" s="14">
         <f>0.7*Y2+0.3*AI2</f>
-        <v>6237240.9249999989</v>
+        <v>5237420</v>
       </c>
       <c r="AC2" s="14">
         <f>0.6*Y2+0.4*AI2</f>
-        <v>6225469.5250000004</v>
+        <v>5237420</v>
       </c>
       <c r="AD2" s="14">
         <f>0.5*Y2+0.5*AI2</f>
-        <v>6213698.125</v>
+        <v>5237420</v>
       </c>
       <c r="AE2" s="14">
         <f>0.4*Y2+0.6*AI2</f>
-        <v>6201926.7249999996</v>
+        <v>5237420</v>
       </c>
       <c r="AF2" s="14">
         <f>0.3*Y2+0.7*AI2</f>
-        <v>6190155.3249999993</v>
+        <v>5237420</v>
       </c>
       <c r="AG2" s="14">
         <f>0.2*Y2+0.8*AI2</f>
-        <v>6178383.9250000007</v>
+        <v>5237420</v>
       </c>
       <c r="AH2" s="14">
         <f>0.1*Y2+0.9*AI2</f>
-        <v>6166612.5250000004</v>
+        <v>5237420</v>
       </c>
       <c r="AI2" s="14">
-        <f>'Texas Data'!E41</f>
-        <v>6154841.125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+        <f>'Texas Data'!E26</f>
+        <v>5237420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>69</v>
       </c>
@@ -3283,7 +2779,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="14">
-        <f t="shared" ref="D2:AI10" si="2">$B3</f>
+        <f t="shared" ref="D3:AI10" si="2">$B3</f>
         <v>0</v>
       </c>
       <c r="T3" s="14">
@@ -3351,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>70</v>
       </c>
@@ -3491,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>71</v>
       </c>
@@ -3631,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>72</v>
       </c>
@@ -3771,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>73</v>
       </c>
@@ -3911,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>74</v>
       </c>
@@ -4051,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>75</v>
       </c>
@@ -4191,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>76</v>
       </c>
@@ -4331,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>77</v>
       </c>
@@ -4477,23 +3973,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L33:L34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -4600,145 +4096,145 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="14">
         <f t="shared" ref="B2:C2" si="0">(C2-D2)+C2</f>
-        <v>707.69142249999993</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="C2" s="14">
         <f t="shared" si="0"/>
-        <v>676.19336499999997</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="D2" s="14">
         <f>(E2-F2)+E2</f>
-        <v>644.69530750000001</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="E2" s="14">
-        <f>'Texas Data'!B28</f>
-        <v>613.19725000000005</v>
+        <f>'Texas Data'!B22</f>
+        <v>986.39450000000011</v>
       </c>
       <c r="F2" s="14">
         <f>0.9*E2+0.1*O2</f>
-        <v>581.69919250000009</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="G2" s="14">
         <f>0.8*E2+0.2*O2</f>
-        <v>550.20113500000002</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="H2" s="14">
         <f>0.7*E2+0.3*O2</f>
-        <v>518.70307750000006</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="I2" s="14">
         <f>0.6*E2+0.4*O2</f>
-        <v>487.20502000000005</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="J2" s="14">
         <f>0.5*E2+0.5*O2</f>
-        <v>455.70696250000003</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="K2" s="14">
         <f>0.4*E2+0.6*O2</f>
-        <v>424.20890500000002</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="L2" s="14">
         <f>0.3*E2+0.7*O2</f>
-        <v>392.7108475</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="M2" s="14">
         <f>0.2*E2+0.8*O2</f>
-        <v>361.21279000000004</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="N2" s="14">
         <f>0.1*E2+0.9*O2</f>
-        <v>329.71473250000003</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="O2" s="14">
-        <f>'Texas Data'!C28</f>
-        <v>298.21667500000001</v>
+        <f>'Texas Data'!C22</f>
+        <v>986.39450000000011</v>
       </c>
       <c r="P2" s="14">
         <f>0.9*O2+0.1*Y2</f>
-        <v>292.10466000000002</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="Q2" s="14">
         <f>0.8*O2+0.2*Y2</f>
-        <v>285.99264500000004</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="R2" s="14">
         <f>0.7*O2+0.3*Y2</f>
-        <v>279.88063</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="S2" s="14">
         <f>0.6*O2+0.4*Y2</f>
-        <v>273.76861500000001</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="T2" s="14">
         <f>0.5*O2+0.5*Y2</f>
-        <v>267.65660000000003</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="U2" s="14">
         <f>0.4*O2+0.6*Y2</f>
-        <v>261.54458499999998</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="V2" s="14">
         <f>0.3*O2+0.7*Y2</f>
-        <v>255.43257</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="W2" s="14">
         <f>0.2*O2+0.8*Y2</f>
-        <v>249.32055500000004</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="X2" s="14">
         <f>0.1*O2+0.9*Y2</f>
-        <v>243.20854000000003</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="Y2" s="14">
-        <f>'Texas Data'!D28</f>
-        <v>237.09652500000001</v>
+        <f>'Texas Data'!D22</f>
+        <v>986.39450000000011</v>
       </c>
       <c r="Z2" s="14">
         <f>0.9*Y2+0.1*AI2</f>
-        <v>234.91798500000002</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AA2" s="14">
         <f>0.8*Y2+0.2*AI2</f>
-        <v>232.73944500000005</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AB2" s="14">
         <f>0.7*Y2+0.3*AI2</f>
-        <v>230.56090499999999</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AC2" s="14">
         <f>0.6*Y2+0.4*AI2</f>
-        <v>228.38236499999999</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AD2" s="14">
         <f>0.5*Y2+0.5*AI2</f>
-        <v>226.20382499999999</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AE2" s="14">
         <f>0.4*Y2+0.6*AI2</f>
-        <v>224.02528500000003</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AF2" s="14">
         <f>0.3*Y2+0.7*AI2</f>
-        <v>221.846745</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AG2" s="14">
         <f>0.2*Y2+0.8*AI2</f>
-        <v>219.66820500000003</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AH2" s="14">
         <f>0.1*Y2+0.9*AI2</f>
-        <v>217.489665</v>
+        <v>986.39450000000011</v>
       </c>
       <c r="AI2" s="14">
-        <f>'Texas Data'!E28</f>
-        <v>215.311125</v>
+        <f>'Texas Data'!E22</f>
+        <v>986.39450000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>